<commit_message>
Edited some incorrect rows of data
</commit_message>
<xml_diff>
--- a/summary_data/series_characteristics.xlsx
+++ b/summary_data/series_characteristics.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrotman/Desktop/septic.shock.data/summary_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39FFD8B-AFB1-274D-BB8D-5339BD05C230}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1F780C-FC1E-8E47-A733-B1378B35E298}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3340" yWindow="2760" windowWidth="27240" windowHeight="16440" xr2:uid="{5CC0EA75-BF82-9846-AD9A-EE5AA3FF34F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -526,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF4CDB4-3875-E947-BFBF-460F355AA8D3}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,7 +540,7 @@
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -572,7 +572,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -601,11 +601,11 @@
         <v>7</v>
       </c>
       <c r="K2">
-        <f>C2+D2</f>
+        <f t="shared" ref="K2:K20" si="0">C2+D2</f>
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -634,11 +634,15 @@
         <v>7</v>
       </c>
       <c r="K3">
-        <f>C3+D3</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M3">
+        <f>K3+K2+K5+K6+K7+K8+K16</f>
+        <v>948</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -667,11 +671,15 @@
         <v>7</v>
       </c>
       <c r="K4">
-        <f>C4+D4</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M4">
+        <f>M3/K21</f>
+        <v>0.5609467455621302</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -700,11 +708,11 @@
         <v>7</v>
       </c>
       <c r="K5">
-        <f>C5+D5</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -733,11 +741,11 @@
         <v>7</v>
       </c>
       <c r="K6">
-        <f>C6+D6</f>
+        <f t="shared" si="0"/>
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -770,11 +778,11 @@
         <v>99</v>
       </c>
       <c r="K7">
-        <f>C7+D7</f>
+        <f t="shared" si="0"/>
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -803,11 +811,11 @@
         <v>7</v>
       </c>
       <c r="K8">
-        <f>C8+D8</f>
+        <f t="shared" si="0"/>
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -836,11 +844,11 @@
         <v>7</v>
       </c>
       <c r="K9">
-        <f>C9+D9</f>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -873,11 +881,11 @@
         <v>12</v>
       </c>
       <c r="K10">
-        <f>C10+D10</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -910,11 +918,11 @@
         <v>52.640000000000008</v>
       </c>
       <c r="K11">
-        <f>C11+D11</f>
+        <f t="shared" si="0"/>
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -947,11 +955,11 @@
         <v>23.85</v>
       </c>
       <c r="K12">
-        <f>C12+D12</f>
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -980,11 +988,11 @@
         <v>7</v>
       </c>
       <c r="K13">
-        <f>C13+D13</f>
+        <f t="shared" si="0"/>
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1013,11 +1021,11 @@
         <v>7</v>
       </c>
       <c r="K14">
-        <f>C14+D14</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1050,11 +1058,11 @@
         <v>53.94</v>
       </c>
       <c r="K15">
-        <f>C15+D15</f>
+        <f t="shared" si="0"/>
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1087,7 +1095,7 @@
         <v>160.07999999999998</v>
       </c>
       <c r="K16">
-        <f>C16+D16</f>
+        <f t="shared" si="0"/>
         <v>276</v>
       </c>
     </row>
@@ -1124,7 +1132,7 @@
         <v>34.720000000000006</v>
       </c>
       <c r="K17">
-        <f>C17+D17</f>
+        <f t="shared" si="0"/>
         <v>62</v>
       </c>
     </row>
@@ -1157,7 +1165,7 @@
         <v>7</v>
       </c>
       <c r="K18">
-        <f>C18+D18</f>
+        <f t="shared" si="0"/>
         <v>105</v>
       </c>
     </row>
@@ -1194,7 +1202,7 @@
         <v>42.339999999999996</v>
       </c>
       <c r="K19">
-        <f>C19+D19</f>
+        <f t="shared" si="0"/>
         <v>73</v>
       </c>
     </row>
@@ -1227,7 +1235,7 @@
         <v>7</v>
       </c>
       <c r="K20">
-        <f>C20+D20</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
     </row>
@@ -1263,5 +1271,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added notebook for figures
</commit_message>
<xml_diff>
--- a/summary_data/series_characteristics.xlsx
+++ b/summary_data/series_characteristics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrotman/Desktop/septic.shock.data/summary_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1F780C-FC1E-8E47-A733-B1378B35E298}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D61FBBD-042A-344E-81D8-52E2DA05A948}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3340" yWindow="2760" windowWidth="27240" windowHeight="16440" xr2:uid="{5CC0EA75-BF82-9846-AD9A-EE5AA3FF34F9}"/>
   </bookViews>
@@ -526,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF4CDB4-3875-E947-BFBF-460F355AA8D3}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,7 +601,7 @@
         <v>7</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K20" si="0">C2+D2</f>
+        <f t="shared" ref="K2:K19" si="0">C2+D2</f>
         <v>123</v>
       </c>
     </row>
@@ -638,8 +638,8 @@
         <v>45</v>
       </c>
       <c r="M3">
-        <f>K3+K2+K5+K6+K7+K8+K16</f>
-        <v>948</v>
+        <f>K3+K2+K5+K6+K7+K8+K15</f>
+        <v>953</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -675,8 +675,8 @@
         <v>70</v>
       </c>
       <c r="M4">
-        <f>M3/K21</f>
-        <v>0.5609467455621302</v>
+        <f>M3/K20</f>
+        <v>0.58038976857490865</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -753,7 +753,7 @@
         <v>18</v>
       </c>
       <c r="C7">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D7">
         <v>94</v>
@@ -775,11 +775,11 @@
       </c>
       <c r="J7">
         <f>I7*K7</f>
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -823,10 +823,10 @@
         <v>14</v>
       </c>
       <c r="C9">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D9">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -924,19 +924,19 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C12">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="D12">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="F12" t="s">
         <v>7</v>
@@ -947,30 +947,30 @@
       <c r="H12" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="1">
-        <v>0.45</v>
-      </c>
-      <c r="J12">
-        <f>I12*K12</f>
-        <v>23.85</v>
+      <c r="I12" t="s">
+        <v>7</v>
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>83</v>
+      </c>
+      <c r="M12">
+        <f>83-37</f>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C13">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D13">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
@@ -989,21 +989,21 @@
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>83</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C14">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="D14">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
@@ -1015,102 +1015,106 @@
         <v>7</v>
       </c>
       <c r="H14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I14" t="s">
-        <v>7</v>
+        <v>40</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="J14">
+        <f>I14*K14</f>
+        <v>53.94</v>
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="D15">
-        <v>51</v>
+        <v>199</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="F15">
+        <v>171</v>
+      </c>
+      <c r="G15">
+        <v>28</v>
+      </c>
+      <c r="H15">
+        <v>3.7</v>
       </c>
       <c r="I15" s="1">
         <v>0.57999999999999996</v>
       </c>
       <c r="J15">
         <f>I15*K15</f>
-        <v>53.94</v>
+        <v>160.07999999999998</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>93</v>
+        <v>276</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C16">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>199</v>
+        <v>62</v>
       </c>
       <c r="E16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16">
-        <v>171</v>
-      </c>
-      <c r="G16">
-        <v>28</v>
-      </c>
-      <c r="H16">
-        <v>3.7</v>
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" t="s">
+        <v>42</v>
       </c>
       <c r="I16" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="J16">
         <f>I16*K16</f>
-        <v>160.07999999999998</v>
+        <v>34.720000000000006</v>
       </c>
       <c r="K16">
         <f t="shared" si="0"/>
-        <v>276</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
@@ -1122,151 +1126,161 @@
         <v>7</v>
       </c>
       <c r="H17" t="s">
-        <v>42</v>
-      </c>
-      <c r="I17" s="1">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="J17">
-        <f>I17*K17</f>
-        <v>34.720000000000006</v>
+        <v>7</v>
+      </c>
+      <c r="I17" t="s">
+        <v>7</v>
       </c>
       <c r="K17">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D18">
-        <v>105</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s">
         <v>7</v>
       </c>
-      <c r="F18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" t="s">
-        <v>7</v>
+      <c r="F18">
+        <v>34</v>
+      </c>
+      <c r="G18">
+        <v>17</v>
       </c>
       <c r="H18" t="s">
-        <v>7</v>
-      </c>
-      <c r="I18" t="s">
-        <v>7</v>
+        <v>45</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="J18">
+        <f>I18*K18</f>
+        <v>42.339999999999996</v>
       </c>
       <c r="K18">
         <f t="shared" si="0"/>
-        <v>105</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C19">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="E19" t="s">
         <v>7</v>
       </c>
-      <c r="F19">
-        <v>34</v>
-      </c>
-      <c r="G19">
-        <v>17</v>
+      <c r="F19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" t="s">
+        <v>7</v>
       </c>
       <c r="H19" t="s">
-        <v>45</v>
-      </c>
-      <c r="I19" s="1">
+        <v>7</v>
+      </c>
+      <c r="I19" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <f>SUM(C2:C19)</f>
+        <v>473</v>
+      </c>
+      <c r="D20">
+        <f>SUM(D2:D19)</f>
+        <v>1169</v>
+      </c>
+      <c r="F20">
+        <f>SUM(F2:F19)</f>
+        <v>389</v>
+      </c>
+      <c r="G20">
+        <f>SUM(G2:G19)</f>
+        <v>83</v>
+      </c>
+      <c r="I20">
+        <f>AVERAGE(I2:I19)</f>
         <v>0.57999999999999996</v>
       </c>
-      <c r="J19">
-        <f>I19*K19</f>
-        <v>42.339999999999996</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="0"/>
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>31</v>
-      </c>
-      <c r="E20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" t="s">
-        <v>7</v>
-      </c>
-      <c r="I20" t="s">
-        <v>7</v>
+      <c r="J20">
+        <f>SUM(J7:J18)/(K7+K10+K11+K14+K15+K16+K18)</f>
+        <v>0.58086294416243656</v>
       </c>
       <c r="K20">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C21">
-        <f>SUM(C2:C20)</f>
-        <v>447</v>
-      </c>
-      <c r="D21">
-        <f>SUM(D2:D20)</f>
-        <v>1243</v>
-      </c>
-      <c r="F21">
-        <f>SUM(F2:F20)</f>
-        <v>389</v>
-      </c>
-      <c r="G21">
-        <f>SUM(G2:G20)</f>
-        <v>83</v>
-      </c>
-      <c r="I21">
-        <f>AVERAGE(I2:I20)</f>
-        <v>0.56374999999999997</v>
-      </c>
-      <c r="J21">
-        <f>SUM(J7:J19)/(K7+K10+K11+K12+K15+K16+K17+K19)</f>
-        <v>0.57245215311004782</v>
-      </c>
-      <c r="K21">
-        <f>SUM(K2:K20)</f>
-        <v>1690</v>
+        <f>SUM(K2:K19)</f>
+        <v>1642</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24">
+        <v>25</v>
+      </c>
+      <c r="D24">
+        <v>28</v>
+      </c>
+      <c r="E24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="J24">
+        <f>I24*K24</f>
+        <v>23.85</v>
+      </c>
+      <c r="K24">
+        <f>C24+D24</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <f>463-25</f>
+        <v>438</v>
+      </c>
+      <c r="D28">
+        <f>1232-D24</f>
+        <v>1204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>